<commit_message>
created pupil_detection and changed canny edge
</commit_message>
<xml_diff>
--- a/Orga/Time_SA.xlsx
+++ b/Orga/Time_SA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Dropbox\My PC (AJP)\Documents\OST\FS2023\SA\Orga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ostch-my.sharepoint.com/personal/anton_paris_ost_ch/Documents/Dokumente/SA/Algorithms_Eye_Detection/Orga/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB916386-7E82-4352-9F31-35D7C3FF6274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{BB916386-7E82-4352-9F31-35D7C3FF6274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FC170F6-CD77-4B43-BA9E-B3C4F8E29BF7}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1980" windowWidth="17280" windowHeight="9072" xr2:uid="{691321FB-2901-46D8-B31E-E0F28A8EDCEA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{691321FB-2901-46D8-B31E-E0F28A8EDCEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -521,21 +521,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -543,9 +528,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -587,9 +569,27 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -610,7 +610,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -908,18 +908,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C67C6AD7-6A08-4079-822A-C94634F4083C}">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="33.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -941,7 +941,7 @@
       <c r="S1" s="4"/>
       <c r="T1" s="4"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -963,7 +963,7 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -985,7 +985,7 @@
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1007,7 +1007,7 @@
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -1031,7 +1031,7 @@
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
@@ -1055,7 +1055,7 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1077,7 +1077,7 @@
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="13" t="s">
         <v>24</v>
@@ -1103,7 +1103,7 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="2"/>
       <c r="C9" s="4"/>
@@ -1123,7 +1123,7 @@
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>1</v>
       </c>
@@ -1133,7 +1133,7 @@
       <c r="C10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="29" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="8" t="s">
@@ -1142,7 +1142,7 @@
       <c r="F10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="29" t="s">
         <v>7</v>
       </c>
       <c r="H10" s="8" t="s">
@@ -1151,7 +1151,7 @@
       <c r="I10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="35" t="s">
+      <c r="J10" s="29" t="s">
         <v>10</v>
       </c>
       <c r="K10" s="8" t="s">
@@ -1160,7 +1160,7 @@
       <c r="L10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="35" t="s">
+      <c r="M10" s="29" t="s">
         <v>13</v>
       </c>
       <c r="N10" s="8" t="s">
@@ -1177,23 +1177,23 @@
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="28"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="22"/>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
       <c r="Q11" s="6"/>
@@ -1201,23 +1201,23 @@
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="15"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="29"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="23"/>
       <c r="O12" s="16"/>
       <c r="P12" s="16"/>
       <c r="Q12" s="6"/>
@@ -1225,23 +1225,23 @@
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="20"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="37"/>
       <c r="H13" s="17"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="29"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="23"/>
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
       <c r="Q13" s="6"/>
@@ -1249,23 +1249,23 @@
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="15"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="29"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="23"/>
       <c r="O14" s="16"/>
       <c r="P14" s="16"/>
       <c r="Q14" s="6"/>
@@ -1273,23 +1273,23 @@
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="15"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="29"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="16"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="29"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="23"/>
       <c r="O15" s="16"/>
       <c r="P15" s="16"/>
       <c r="Q15" s="6"/>
@@ -1297,22 +1297,22 @@
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="15"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="37"/>
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
       <c r="P16" s="16"/>
@@ -1321,23 +1321,23 @@
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="15"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="37"/>
       <c r="O17" s="16"/>
       <c r="P17" s="16"/>
       <c r="Q17" s="6"/>
@@ -1345,101 +1345,101 @@
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="20"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="37"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="15"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="38" t="s">
+      <c r="C19" s="21"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="P19" s="39"/>
+      <c r="P19" s="33"/>
       <c r="Q19" s="7"/>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="23">
+      <c r="B20" s="18">
         <v>1</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="20">
         <v>2</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20" s="28">
         <v>3</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="19">
         <v>4</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="20">
         <v>5</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="28">
         <v>6</v>
       </c>
-      <c r="H20" s="24">
+      <c r="H20" s="19">
         <v>7</v>
       </c>
-      <c r="I20" s="25">
+      <c r="I20" s="20">
         <v>8</v>
       </c>
-      <c r="J20" s="34">
+      <c r="J20" s="28">
         <v>9</v>
       </c>
-      <c r="K20" s="24">
+      <c r="K20" s="19">
         <v>10</v>
       </c>
-      <c r="L20" s="25">
+      <c r="L20" s="20">
         <v>11</v>
       </c>
-      <c r="M20" s="34">
+      <c r="M20" s="28">
         <v>12</v>
       </c>
-      <c r="N20" s="24">
+      <c r="N20" s="19">
         <v>13</v>
       </c>
-      <c r="O20" s="25">
+      <c r="O20" s="20">
         <v>14</v>
       </c>
-      <c r="P20" s="25">
+      <c r="P20" s="20">
         <v>15</v>
       </c>
       <c r="Q20" s="7"/>
@@ -1447,28 +1447,28 @@
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="36" t="s">
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="36" t="s">
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="36" t="s">
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N21" s="4"/>
@@ -1479,7 +1479,7 @@
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1501,7 +1501,7 @@
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1523,7 +1523,7 @@
       <c r="S23" s="4"/>
       <c r="T23" s="4"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1545,7 +1545,7 @@
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1567,7 +1567,7 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1589,7 +1589,7 @@
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1611,7 +1611,7 @@
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1633,7 +1633,7 @@
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1655,7 +1655,7 @@
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1677,7 +1677,7 @@
       <c r="S30" s="4"/>
       <c r="T30" s="4"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1699,7 +1699,7 @@
       <c r="S31" s="4"/>
       <c r="T31" s="4"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1721,7 +1721,7 @@
       <c r="S32" s="4"/>
       <c r="T32" s="4"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1743,7 +1743,7 @@
       <c r="S33" s="4"/>
       <c r="T33" s="4"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1765,7 +1765,7 @@
       <c r="S34" s="4"/>
       <c r="T34" s="4"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1787,7 +1787,7 @@
       <c r="S35" s="4"/>
       <c r="T35" s="4"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1809,7 +1809,7 @@
       <c r="S36" s="4"/>
       <c r="T36" s="4"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1831,7 +1831,7 @@
       <c r="S37" s="4"/>
       <c r="T37" s="4"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1853,7 +1853,7 @@
       <c r="S38" s="4"/>
       <c r="T38" s="4"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1875,7 +1875,7 @@
       <c r="S39" s="4"/>
       <c r="T39" s="4"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1897,7 +1897,7 @@
       <c r="S40" s="4"/>
       <c r="T40" s="4"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1919,7 +1919,7 @@
       <c r="S41" s="4"/>
       <c r="T41" s="4"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1941,7 +1941,7 @@
       <c r="S42" s="4"/>
       <c r="T42" s="4"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1963,7 +1963,7 @@
       <c r="S43" s="4"/>
       <c r="T43" s="4"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1985,7 +1985,7 @@
       <c r="S44" s="4"/>
       <c r="T44" s="4"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2007,7 +2007,7 @@
       <c r="S45" s="4"/>
       <c r="T45" s="4"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2029,7 +2029,7 @@
       <c r="S46" s="4"/>
       <c r="T46" s="4"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2051,7 +2051,7 @@
       <c r="S47" s="4"/>
       <c r="T47" s="4"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2073,7 +2073,7 @@
       <c r="S48" s="4"/>
       <c r="T48" s="4"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2095,7 +2095,7 @@
       <c r="S49" s="4"/>
       <c r="T49" s="4"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2117,7 +2117,7 @@
       <c r="S50" s="4"/>
       <c r="T50" s="4"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2139,7 +2139,7 @@
       <c r="S51" s="4"/>
       <c r="T51" s="4"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -2161,7 +2161,7 @@
       <c r="S52" s="4"/>
       <c r="T52" s="4"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -2183,7 +2183,7 @@
       <c r="S53" s="4"/>
       <c r="T53" s="4"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -2205,7 +2205,7 @@
       <c r="S54" s="4"/>
       <c r="T54" s="4"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -2227,7 +2227,7 @@
       <c r="S55" s="4"/>
       <c r="T55" s="4"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -2249,7 +2249,7 @@
       <c r="S56" s="4"/>
       <c r="T56" s="4"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2271,7 +2271,7 @@
       <c r="S57" s="4"/>
       <c r="T57" s="4"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -2293,7 +2293,7 @@
       <c r="S58" s="4"/>
       <c r="T58" s="4"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -2315,7 +2315,7 @@
       <c r="S59" s="4"/>
       <c r="T59" s="4"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C60" s="5"/>
     </row>
   </sheetData>

</xml_diff>